<commit_message>
update impfzahlen corona report
</commit_message>
<xml_diff>
--- a/data/kbvreport_export/faktenblatttabellen_2021-02-07.xlsx
+++ b/data/kbvreport_export/faktenblatttabellen_2021-02-07.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="354">
   <si>
     <t xml:space="preserve">Testungen</t>
   </si>
@@ -354,94 +354,94 @@
     <t xml:space="preserve">Todesfälle &amp; Sterblichkeit</t>
   </si>
   <si>
-    <t xml:space="preserve">KW 1</t>
+    <t xml:space="preserve">KW 2</t>
   </si>
   <si>
     <t xml:space="preserve">0 bis 59 Jahre</t>
   </si>
   <si>
-    <t xml:space="preserve">130 ( 0,2%)</t>
-  </si>
-  <si>
     <t xml:space="preserve">126 ( 0,1%)</t>
   </si>
   <si>
-    <t xml:space="preserve">  -3,1%</t>
+    <t xml:space="preserve">95 ( 0,1%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-24,6%</t>
   </si>
   <si>
     <t xml:space="preserve">60 bis 79 Jahre</t>
   </si>
   <si>
-    <t xml:space="preserve">1244 ( 5,6%)</t>
-  </si>
-  <si>
     <t xml:space="preserve">1219 ( 4,9%)</t>
   </si>
   <si>
-    <t xml:space="preserve">  -2,0%</t>
+    <t xml:space="preserve">904 ( 4,5%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-25,8%</t>
   </si>
   <si>
     <t xml:space="preserve">80 Jahre +</t>
   </si>
   <si>
-    <t xml:space="preserve">3695 (21,1%)</t>
-  </si>
-  <si>
     <t xml:space="preserve">3553 (18,5%)</t>
   </si>
   <si>
-    <t xml:space="preserve">  -3,8%</t>
+    <t xml:space="preserve">2998 (17,3%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-15,6%</t>
   </si>
   <si>
     <t xml:space="preserve">Gesamt</t>
   </si>
   <si>
-    <t xml:space="preserve">5072 ( 4,1%)</t>
-  </si>
-  <si>
     <t xml:space="preserve">4902 ( 3,4%)</t>
   </si>
   <si>
-    <t xml:space="preserve">  -3,4%</t>
+    <t xml:space="preserve">4002 ( 3,4%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-18,4%</t>
   </si>
   <si>
     <t xml:space="preserve">Übersterblichkeit</t>
   </si>
   <si>
-    <t xml:space="preserve">137 ( 8,4%)</t>
-  </si>
-  <si>
     <t xml:space="preserve">-120 (-6,6%)</t>
   </si>
   <si>
-    <t xml:space="preserve">-187,6%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1136 (18,1%)</t>
+    <t xml:space="preserve">-23 (-1,3%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-80,8%</t>
   </si>
   <si>
     <t xml:space="preserve">674 (10,2%)</t>
   </si>
   <si>
-    <t xml:space="preserve"> -40,7%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5097 (47,5%)</t>
+    <t xml:space="preserve">586 ( 8,7%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-13,1%</t>
   </si>
   <si>
     <t xml:space="preserve">4436 (40,6%)</t>
   </si>
   <si>
-    <t xml:space="preserve"> -13,0%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6370 (34,2%)</t>
+    <t xml:space="preserve">3839 (34,7%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-13,5%</t>
   </si>
   <si>
     <t xml:space="preserve">4990 (25,8%)</t>
   </si>
   <si>
-    <t xml:space="preserve"> -21,7%</t>
+    <t xml:space="preserve">4402 (22,4%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-11,8%</t>
   </si>
   <si>
     <t xml:space="preserve">Vorwarnzeit</t>
@@ -790,61 +790,61 @@
     <t xml:space="preserve">Geimpfte Personen</t>
   </si>
   <si>
-    <t xml:space="preserve">Stand 9.2.</t>
+    <t xml:space="preserve">Stand 10.2.</t>
   </si>
   <si>
     <t xml:space="preserve">Gesamt-Bevölkerung</t>
   </si>
   <si>
-    <t xml:space="preserve">2344802 ( 2,8 %)</t>
+    <t xml:space="preserve">2405156 ( 2,9 %)</t>
   </si>
   <si>
     <t xml:space="preserve">Mit nur 1 Impfung</t>
   </si>
   <si>
-    <t xml:space="preserve">1320171 ( 1,6 %)</t>
+    <t xml:space="preserve">1300662 ( 1,6 %)</t>
   </si>
   <si>
     <t xml:space="preserve">Mit 2 Impfungen</t>
   </si>
   <si>
-    <t xml:space="preserve">1024631 ( 1,2 %)</t>
+    <t xml:space="preserve">1104494 ( 1,3 %)</t>
   </si>
   <si>
     <t xml:space="preserve">Pflegeheimbewohnende</t>
   </si>
   <si>
-    <t xml:space="preserve">657328 (82,7 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">340358 (42,8 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">316970 (39,9 %)</t>
+    <t xml:space="preserve">666234 (83,8 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">301092 (37,9 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">365142 (45,9 %)</t>
   </si>
   <si>
     <t xml:space="preserve">Über-80-Jährige</t>
   </si>
   <si>
-    <t xml:space="preserve">830292 (14,6 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">506033 ( 8,9 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">324259 ( 5,7 %)</t>
+    <t xml:space="preserve">861298 (15,2 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">486386 ( 8,6 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">374912 ( 6,6 %)</t>
   </si>
   <si>
     <t xml:space="preserve">Personal in ...</t>
   </si>
   <si>
-    <t xml:space="preserve">1101480 (30,6 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">584358 (16,2 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">517122 (14,4 %)</t>
+    <t xml:space="preserve">1124283 (31,2 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">594677 (16,5 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">529606 (14,7 %)</t>
   </si>
   <si>
     <t xml:space="preserve">Gesamt nur 1x</t>
@@ -874,208 +874,223 @@
     <t xml:space="preserve">1,6</t>
   </si>
   <si>
+    <t xml:space="preserve">1,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">57,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">46,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">61,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">44,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">46,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1,7</t>
+  </si>
+  <si>
     <t xml:space="preserve">1,2</t>
   </si>
   <si>
-    <t xml:space="preserve">42,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">39,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 8,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,0</t>
-  </si>
-  <si>
     <t xml:space="preserve">39,1</t>
   </si>
   <si>
-    <t xml:space="preserve">22,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 9,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">56,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 9,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 8,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">79,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17,4</t>
+    <t xml:space="preserve">44,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">62,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3,5</t>
   </si>
   <si>
     <t xml:space="preserve">1,9</t>
   </si>
   <si>
-    <t xml:space="preserve">49,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">42,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">57,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 7,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">41,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 8,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">44,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15,2</t>
+    <t xml:space="preserve">60,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">41,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">44,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">58,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30,7</t>
   </si>
   <si>
     <t xml:space="preserve"> 3,8</t>
   </si>
   <si>
-    <t xml:space="preserve">2,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">62,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">39,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">42,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">58,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 9,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 7,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">42,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">58,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12,6</t>
+    <t xml:space="preserve">10,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5,2</t>
   </si>
 </sst>
 </file>
@@ -1551,10 +1566,10 @@
         <v>284</v>
       </c>
       <c r="F2" t="s">
-        <v>249</v>
+        <v>285</v>
       </c>
       <c r="G2" t="n">
-        <v>3369433</v>
+        <v>3509650</v>
       </c>
       <c r="H2" t="n">
         <v>69</v>
@@ -1568,22 +1583,22 @@
         <v>280</v>
       </c>
       <c r="B3" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C3" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D3" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E3" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="F3" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="G3" t="n">
-        <v>405844</v>
+        <v>421144</v>
       </c>
       <c r="H3" t="n">
         <v>58</v>
@@ -1594,25 +1609,25 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B4" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="C4" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D4" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E4" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="F4" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="G4" t="n">
-        <v>596841</v>
+        <v>614925</v>
       </c>
       <c r="H4" t="n">
         <v>70</v>
@@ -1623,25 +1638,25 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B5" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="C5" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D5" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E5" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="F5" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="G5" t="n">
-        <v>175502</v>
+        <v>179863</v>
       </c>
       <c r="H5" t="n">
         <v>59</v>
@@ -1652,7 +1667,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B6" t="s">
         <v>281</v>
@@ -1664,13 +1679,13 @@
         <v>302</v>
       </c>
       <c r="E6" t="s">
-        <v>234</v>
+        <v>303</v>
       </c>
       <c r="F6" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="G6" t="n">
-        <v>109452</v>
+        <v>113127</v>
       </c>
       <c r="H6" t="n">
         <v>79</v>
@@ -1681,25 +1696,25 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B7" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="C7" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D7" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="E7" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F7" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="G7" t="n">
-        <v>32424</v>
+        <v>33421</v>
       </c>
       <c r="H7" t="n">
         <v>72</v>
@@ -1710,25 +1725,25 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B8" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C8" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D8" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E8" t="s">
-        <v>312</v>
+        <v>234</v>
       </c>
       <c r="F8" t="s">
         <v>313</v>
       </c>
       <c r="G8" t="n">
-        <v>80326</v>
+        <v>83752</v>
       </c>
       <c r="H8" t="n">
         <v>68</v>
@@ -1742,10 +1757,10 @@
         <v>280</v>
       </c>
       <c r="B9" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C9" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D9" t="s">
         <v>314</v>
@@ -1757,7 +1772,7 @@
         <v>316</v>
       </c>
       <c r="G9" t="n">
-        <v>230477</v>
+        <v>239310</v>
       </c>
       <c r="H9" t="n">
         <v>73</v>
@@ -1771,22 +1786,22 @@
         <v>317</v>
       </c>
       <c r="B10" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="C10" t="s">
+        <v>293</v>
+      </c>
+      <c r="D10" t="s">
         <v>318</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>319</v>
-      </c>
-      <c r="E10" t="s">
-        <v>284</v>
       </c>
       <c r="F10" t="s">
         <v>320</v>
       </c>
       <c r="G10" t="n">
-        <v>85709</v>
+        <v>89006</v>
       </c>
       <c r="H10" t="n">
         <v>77</v>
@@ -1797,7 +1812,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>281</v>
+        <v>321</v>
       </c>
       <c r="B11" t="s">
         <v>321</v>
@@ -1815,7 +1830,7 @@
         <v>325</v>
       </c>
       <c r="G11" t="n">
-        <v>273061</v>
+        <v>279784</v>
       </c>
       <c r="H11" t="n">
         <v>63</v>
@@ -1826,25 +1841,25 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>290</v>
+        <v>310</v>
       </c>
       <c r="B12" t="s">
-        <v>321</v>
+        <v>281</v>
       </c>
       <c r="C12" t="s">
         <v>326</v>
       </c>
       <c r="D12" t="s">
-        <v>310</v>
+        <v>327</v>
       </c>
       <c r="E12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="F12" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="G12" t="n">
-        <v>659512</v>
+        <v>705386</v>
       </c>
       <c r="H12" t="n">
         <v>67</v>
@@ -1855,25 +1870,25 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B13" t="s">
-        <v>290</v>
+        <v>309</v>
       </c>
       <c r="C13" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D13" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E13" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="F13" t="s">
-        <v>284</v>
+        <v>334</v>
       </c>
       <c r="G13" t="n">
-        <v>207606</v>
+        <v>216076</v>
       </c>
       <c r="H13" t="n">
         <v>59</v>
@@ -1884,25 +1899,25 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>321</v>
+        <v>286</v>
       </c>
       <c r="B14" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="C14" t="s">
-        <v>312</v>
+        <v>335</v>
       </c>
       <c r="D14" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="E14" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="F14" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="G14" t="n">
-        <v>40837</v>
+        <v>41770</v>
       </c>
       <c r="H14" t="n">
         <v>102</v>
@@ -1919,19 +1934,19 @@
         <v>321</v>
       </c>
       <c r="C15" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="D15" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="E15" t="s">
-        <v>316</v>
+        <v>341</v>
       </c>
       <c r="F15" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="G15" t="n">
-        <v>156889</v>
+        <v>164454</v>
       </c>
       <c r="H15" t="n">
         <v>79</v>
@@ -1942,25 +1957,25 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>309</v>
+        <v>321</v>
       </c>
       <c r="B16" t="s">
-        <v>339</v>
+        <v>291</v>
       </c>
       <c r="C16" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D16" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="E16" t="s">
-        <v>342</v>
+        <v>249</v>
       </c>
       <c r="F16" t="s">
-        <v>303</v>
+        <v>249</v>
       </c>
       <c r="G16" t="n">
-        <v>88726</v>
+        <v>90979</v>
       </c>
       <c r="H16" t="n">
         <v>96</v>
@@ -1971,25 +1986,25 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B17" t="s">
-        <v>281</v>
+        <v>310</v>
       </c>
       <c r="C17" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="D17" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="E17" t="s">
-        <v>324</v>
+        <v>348</v>
       </c>
       <c r="F17" t="s">
-        <v>289</v>
+        <v>349</v>
       </c>
       <c r="G17" t="n">
-        <v>134814</v>
+        <v>139640</v>
       </c>
       <c r="H17" t="n">
         <v>60</v>
@@ -2000,25 +2015,25 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>329</v>
+        <v>345</v>
       </c>
       <c r="B18" t="s">
         <v>321</v>
       </c>
       <c r="C18" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="D18" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="E18" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="F18" t="s">
-        <v>324</v>
+        <v>353</v>
       </c>
       <c r="G18" t="n">
-        <v>91413</v>
+        <v>97013</v>
       </c>
       <c r="H18" t="n">
         <v>125</v>

</xml_diff>